<commit_message>
updating and organizing runs
</commit_message>
<xml_diff>
--- a/Adriatic/Adriatic_v8_age5_hake.xlsx
+++ b/Adriatic/Adriatic_v8_age5_hake.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27075" windowHeight="10710" firstSheet="14" activeTab="24"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27075" windowHeight="10710" firstSheet="14" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -7784,8 +7784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14090,7 +14090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>

</xml_diff>